<commit_message>
11.12 read a paper
</commit_message>
<xml_diff>
--- a/PaperNotes.xlsx
+++ b/PaperNotes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\学习\论文\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\学习\论文\PapersNote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD306E5-5FB5-4243-B683-4536892AD296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44190496-3155-45A7-AB1E-E1E7CF0BFE53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="over-smooth等" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>摘要</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>Composition-based Multi-Relational Graph Convolutional Networks</t>
-  </si>
-  <si>
-    <t>https://github.com/malllabiisc/CompGCN</t>
   </si>
   <si>
     <t>多关系图；有向图</t>
@@ -543,13 +540,36 @@
       </rPr>
       <t>模型。</t>
     </r>
+  </si>
+  <si>
+    <t>Hypergraph Neural Networks</t>
+  </si>
+  <si>
+    <t>AAAI 2019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/iMoonLab/HGNN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/malllabiisc/CompGCN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超图，即一条边连接多个节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究超图上高阶的数据关联性；处理多模态数据缓解传统的超图学习方法具有高计算复杂度以及存储损失的问题。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,6 +733,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="1"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -736,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -763,44 +790,47 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1091,47 +1121,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.58203125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="62.08203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="11.75" style="13" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="27.08203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="23.4140625" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="13"/>
+    <col min="1" max="1" width="5.58203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="62.08203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.75" style="12" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="27.08203125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="23.4140625" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="A1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>27</v>
+      <c r="F2" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1141,37 +1171,37 @@
         <v>3</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="4" spans="1:6" ht="73" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="31" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1181,13 +1211,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
@@ -1205,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E297E202-346B-42B2-96E2-219E751E9F2C}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.3"/>
@@ -1222,37 +1252,37 @@
     <col min="7" max="16384" width="8.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>4</v>
       </c>
@@ -1263,16 +1293,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="78.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="62" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>5</v>
       </c>
@@ -1303,13 +1333,33 @@
         <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1317,12 +1367,8 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="https://github.com/chennnM/GCNII" xr:uid="{2C030EC8-0398-4877-BC7E-EC2DBF7D46F0}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{FE9722AC-4744-4E45-8BBA-F75780ECD713}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1336,90 +1382,90 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="13"/>
-    <col min="2" max="2" width="46.5" style="13" customWidth="1"/>
-    <col min="3" max="3" width="13" style="13" customWidth="1"/>
-    <col min="4" max="4" width="34.5" style="13" customWidth="1"/>
-    <col min="5" max="5" width="36.75" style="13" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" style="13" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="13"/>
+    <col min="1" max="1" width="8.6640625" style="12"/>
+    <col min="2" max="2" width="46.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13" style="12" customWidth="1"/>
+    <col min="4" max="4" width="34.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="36.75" style="12" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="A1" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>27</v>
+      <c r="F2" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="108.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="77.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="77.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
-        <v>9</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="5" spans="1:6" ht="20.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="22"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="9"/>
-      <c r="F5" s="21"/>
+      <c r="F5" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1435,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365F3F5E-AD18-4087-94AC-231FF58C9EEB}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1451,33 +1497,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="A1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>27</v>
+      <c r="F2" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="92" x14ac:dyDescent="0.35">
@@ -1485,18 +1531,18 @@
         <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="24"/>
+      <c r="E3" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B4" s="9"/>

</xml_diff>